<commit_message>
Updating with final proyect complete
</commit_message>
<xml_diff>
--- a/docs/DisenoETL.xlsx
+++ b/docs/DisenoETL.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dhoyoso\Documents\Maestria UNIANDES\Cursos\APRENDIZAJE NO SUPERVISADO\Proyecto\MarketSegInsurancePayAsYouDrive\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{118384D8-2344-47C5-A4D0-B18D0B5BD497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29B46EA8-4D9F-453B-BCD5-AB5E9859AB93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PlantillaDiseñoETL" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja1" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,10 +36,400 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="149">
+  <si>
+    <t>Fuente de datos 1:</t>
+  </si>
+  <si>
+    <t>Fuente de datos 2:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Extraer información de </t>
+  </si>
+  <si>
+    <t>Campos a incluir:</t>
+  </si>
+  <si>
+    <t>2. Transformaciones</t>
+  </si>
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>3. Carga de los datos</t>
+  </si>
+  <si>
+    <t>Destino de los datos:</t>
+  </si>
+  <si>
+    <t>Campos a cargar:</t>
+  </si>
+  <si>
+    <t>* Tabla CONDUCTORES</t>
+  </si>
+  <si>
+    <t>* Tabla VICTIMAS</t>
+  </si>
+  <si>
+    <t>* Tabla ACCIDENTES</t>
+  </si>
+  <si>
+    <t>1. CONDUCTORES_AGG</t>
+  </si>
+  <si>
+    <t>2. ACCIDENTES_AGG</t>
+  </si>
+  <si>
+    <t>idFormulario</t>
+  </si>
+  <si>
+    <t>MES_PROCESADO</t>
+  </si>
+  <si>
+    <t>DIA_PROCESADO</t>
+  </si>
+  <si>
+    <t>EDAD_PROCESADA</t>
+  </si>
+  <si>
+    <t>LLevaCinturon</t>
+  </si>
+  <si>
+    <t>LLevaChaleco</t>
+  </si>
+  <si>
+    <t>LLevaCasco</t>
+  </si>
+  <si>
+    <t>Sexo</t>
+  </si>
+  <si>
+    <t>GRAVEDAD_PROCESADA</t>
+  </si>
+  <si>
+    <t>PortaLicencia</t>
+  </si>
+  <si>
+    <t>CodigoCategoriaLicencia</t>
+  </si>
+  <si>
+    <t>CodigoRestriccionLicencia</t>
+  </si>
+  <si>
+    <t>OficinaExpedicionLicencia</t>
+  </si>
+  <si>
+    <t>EsPropietarioVehiculo</t>
+  </si>
+  <si>
+    <t>ModeloVehiculo</t>
+  </si>
+  <si>
+    <t>CapacidadCarga</t>
+  </si>
+  <si>
+    <t>CantidadPasajeros</t>
+  </si>
+  <si>
+    <t>ClaseVehiculo</t>
+  </si>
+  <si>
+    <t>ServicioVehiculo</t>
+  </si>
+  <si>
+    <t>ModalidadVehiculo</t>
+  </si>
+  <si>
+    <t>PosseSeguroResponsabilidad</t>
+  </si>
+  <si>
+    <t>TipoFalla</t>
+  </si>
+  <si>
+    <t>VEHICULO_VIAJABA_CLASIFICADO</t>
+  </si>
+  <si>
+    <t>Dia</t>
+  </si>
+  <si>
+    <t>Oficina</t>
+  </si>
+  <si>
+    <t>GravedadCod</t>
+  </si>
+  <si>
+    <t>GravedadNombre</t>
+  </si>
+  <si>
+    <t>ClaseCodigo</t>
+  </si>
+  <si>
+    <t>ClaseNombre</t>
+  </si>
+  <si>
+    <t>ChoqueCodigo</t>
+  </si>
+  <si>
+    <t>ChoqueNombre</t>
+  </si>
+  <si>
+    <t>ObjetoFijoCodigo</t>
+  </si>
+  <si>
+    <t>ObjetoFijoNombre</t>
+  </si>
+  <si>
+    <t>OtraClase</t>
+  </si>
+  <si>
+    <t>NombreOtraClase</t>
+  </si>
+  <si>
+    <t>Latitud</t>
+  </si>
+  <si>
+    <t>Longitud</t>
+  </si>
+  <si>
+    <t>Direccion</t>
+  </si>
+  <si>
+    <t>TipoVia1</t>
+  </si>
+  <si>
+    <t>NumeroVia1</t>
+  </si>
+  <si>
+    <t>LetraVia1</t>
+  </si>
+  <si>
+    <t>CardinalVia1</t>
+  </si>
+  <si>
+    <t>TipoVia2</t>
+  </si>
+  <si>
+    <t>NumeroVia2</t>
+  </si>
+  <si>
+    <t>LetraVia2</t>
+  </si>
+  <si>
+    <t>CardinalVia2</t>
+  </si>
+  <si>
+    <t>Complemento</t>
+  </si>
+  <si>
+    <t>Municipio</t>
+  </si>
+  <si>
+    <t>Localidad</t>
+  </si>
+  <si>
+    <t>FechaOcurrencia</t>
+  </si>
+  <si>
+    <t>HoraOcurrencia</t>
+  </si>
+  <si>
+    <t>HORA_PROCESADA</t>
+  </si>
+  <si>
+    <t>Sector</t>
+  </si>
+  <si>
+    <t>Zona</t>
+  </si>
+  <si>
+    <t>TipoDisenno</t>
+  </si>
+  <si>
+    <t>TipoTiempo</t>
+  </si>
+  <si>
+    <t>ZonaTransito</t>
+  </si>
+  <si>
+    <t>AreaTransito</t>
+  </si>
+  <si>
+    <t>CON_BICICLETA</t>
+  </si>
+  <si>
+    <t>CON_CARGA</t>
+  </si>
+  <si>
+    <t>CON_EMBRIAGUEZ</t>
+  </si>
+  <si>
+    <t>CON_HUECOS</t>
+  </si>
+  <si>
+    <t>CON_MENORES</t>
+  </si>
+  <si>
+    <t>CON_MOTO</t>
+  </si>
+  <si>
+    <t>CON_PEATON</t>
+  </si>
+  <si>
+    <t>CON_PERSONA_MAYOR</t>
+  </si>
+  <si>
+    <t>CON_RUTAS</t>
+  </si>
+  <si>
+    <t>CON_TPI</t>
+  </si>
+  <si>
+    <t>CON_VELOCIDAD</t>
+  </si>
+  <si>
+    <t>Vehiculo</t>
+  </si>
+  <si>
+    <t>ClaseOficial</t>
+  </si>
+  <si>
+    <t>GradoOficial</t>
+  </si>
+  <si>
+    <t>UnidadOficial</t>
+  </si>
+  <si>
+    <t>EstabaServicioOficial</t>
+  </si>
+  <si>
+    <t>FechaExpedicion</t>
+  </si>
+  <si>
+    <t>RadioAccion</t>
+  </si>
+  <si>
+    <t>Numero</t>
+  </si>
+  <si>
+    <t>LlevaChaleco</t>
+  </si>
+  <si>
+    <t>Peaton_Pasajero</t>
+  </si>
+  <si>
+    <t>CodigoVehiculo</t>
+  </si>
+  <si>
+    <t>EstabaEnServicio</t>
+  </si>
+  <si>
+    <t>Trasladado_en</t>
+  </si>
+  <si>
+    <t>VEHICULO_VIAJABA</t>
+  </si>
+  <si>
+    <t>Fuente de datos 3:</t>
+  </si>
+  <si>
+    <t>* Tabla CONDUCTORES_AGG</t>
+  </si>
+  <si>
+    <t>* IdConductor</t>
+  </si>
+  <si>
+    <t>* Sexo</t>
+  </si>
+  <si>
+    <t>* PortaLicencia</t>
+  </si>
+  <si>
+    <t>* CodigoCategoriaLicencia</t>
+  </si>
+  <si>
+    <t>* CodigoRestriccionLicencia</t>
+  </si>
+  <si>
+    <t>* ModeloVehiculo</t>
+  </si>
+  <si>
+    <t>* CapacidadCarga</t>
+  </si>
+  <si>
+    <t>* CantidadPasajeros</t>
+  </si>
+  <si>
+    <t>* ClaseVehiculo</t>
+  </si>
+  <si>
+    <t>* VehiculoViajabaClasificado</t>
+  </si>
+  <si>
+    <t>* Edad</t>
+  </si>
+  <si>
+    <t>* Gravedad</t>
+  </si>
+  <si>
+    <t>* ServicioVehiculo</t>
+  </si>
+  <si>
+    <t>* PosseSeguroResponsabilidad</t>
+  </si>
+  <si>
+    <t>* HuboFallaVehiculo</t>
+  </si>
+  <si>
+    <t>* CON_BICICLETA</t>
+  </si>
+  <si>
+    <t>* CON_CARGA</t>
+  </si>
+  <si>
+    <t>* CON_EMBRIAGUEZ</t>
+  </si>
+  <si>
+    <t>* CON_HUECOS</t>
+  </si>
+  <si>
+    <t>* CON_MENORES</t>
+  </si>
+  <si>
+    <t>* CON_MOTO</t>
+  </si>
+  <si>
+    <t>* CON_PEATON</t>
+  </si>
+  <si>
+    <t>* CON_PERSONA_MAYOR</t>
+  </si>
+  <si>
+    <t>* CON_RUTAS</t>
+  </si>
+  <si>
+    <t>* CON_TPI</t>
+  </si>
+  <si>
+    <t>* CON_VELOCIDAD</t>
+  </si>
+  <si>
+    <t>* CantidadVictimas</t>
+  </si>
+  <si>
+    <t>* CantidadVictimasPeatones</t>
+  </si>
+  <si>
+    <t>* CantidadVictimasAcompanante</t>
+  </si>
+  <si>
+    <t>* CantidadVictimasPasajeros</t>
+  </si>
   <si>
     <r>
-      <t xml:space="preserve">Diseño ETL Incremental: </t>
+      <t xml:space="preserve">Diseño ETL: </t>
     </r>
     <r>
       <rPr>
@@ -51,318 +440,69 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>RaSa - Grupo 7</t>
+      <t>Aprendizaje No Supervisado - Grupo 5</t>
     </r>
   </si>
   <si>
-    <t>Fuente de datos 1:</t>
-  </si>
-  <si>
-    <t>Fuente de datos 2:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Extraer información de </t>
-  </si>
-  <si>
-    <t>Fuente de datos:</t>
-  </si>
-  <si>
-    <t>Campos a incluir:</t>
-  </si>
-  <si>
-    <t>* Fecha</t>
-  </si>
-  <si>
-    <t>IdAreaDeServicio_T</t>
-  </si>
-  <si>
-    <t>IdGeografia_T</t>
-  </si>
-  <si>
-    <t>IdAreaDeServicio_DWH</t>
-  </si>
-  <si>
-    <t>IdGeografia_DWH</t>
-  </si>
-  <si>
-    <t>2. Transformaciones</t>
-  </si>
-  <si>
-    <t>Fecha</t>
-  </si>
-  <si>
-    <t>Area</t>
-  </si>
-  <si>
-    <t>3. Carga de los datos</t>
-  </si>
-  <si>
-    <t>Destino de los datos:</t>
-  </si>
-  <si>
-    <t>* Tabla AsociacionAreaServicioGeografia</t>
-  </si>
-  <si>
-    <t>Campos a cargar:</t>
-  </si>
-  <si>
-    <t>* Tabla Fecha</t>
-  </si>
-  <si>
-    <t>* IdFecha</t>
-  </si>
-  <si>
-    <t>* Dia</t>
-  </si>
-  <si>
-    <t>* Mes</t>
-  </si>
-  <si>
-    <t>* Annio</t>
-  </si>
-  <si>
-    <t>* Tabla CONDUCTORES</t>
-  </si>
-  <si>
-    <t>* Tabla VICTIMAS</t>
-  </si>
-  <si>
-    <t>* Tabla ACCIDENTES</t>
-  </si>
-  <si>
-    <t>1. CONDUCTORES_AGG</t>
-  </si>
-  <si>
-    <t>2. ACCIDENTES_AGG</t>
-  </si>
-  <si>
-    <t>idFormulario</t>
-  </si>
-  <si>
-    <t>non-null</t>
-  </si>
-  <si>
-    <t>int64</t>
-  </si>
-  <si>
-    <t>datetime64[ns]</t>
-  </si>
-  <si>
-    <t>MES_PROCESADO</t>
-  </si>
-  <si>
-    <t>object</t>
-  </si>
-  <si>
-    <t>DIA_PROCESADO</t>
-  </si>
-  <si>
-    <t>EDAD_PROCESADA</t>
-  </si>
-  <si>
-    <t>LLevaCinturon</t>
-  </si>
-  <si>
-    <t>LLevaChaleco</t>
-  </si>
-  <si>
-    <t>LLevaCasco</t>
-  </si>
-  <si>
-    <t>Sexo</t>
-  </si>
-  <si>
-    <t>GRAVEDAD_PROCESADA</t>
-  </si>
-  <si>
-    <t>PortaLicencia</t>
-  </si>
-  <si>
-    <t>CodigoCategoriaLicencia</t>
-  </si>
-  <si>
-    <t>CodigoRestriccionLicencia</t>
-  </si>
-  <si>
-    <t>OficinaExpedicionLicencia</t>
-  </si>
-  <si>
-    <t>EsPropietarioVehiculo</t>
-  </si>
-  <si>
-    <t>ModeloVehiculo</t>
-  </si>
-  <si>
-    <t>float64</t>
-  </si>
-  <si>
-    <t>CapacidadCarga</t>
-  </si>
-  <si>
-    <t>CantidadPasajeros</t>
-  </si>
-  <si>
-    <t>ClaseVehiculo</t>
-  </si>
-  <si>
-    <t>ServicioVehiculo</t>
-  </si>
-  <si>
-    <t>ModalidadVehiculo</t>
-  </si>
-  <si>
-    <t>PosseSeguroResponsabilidad</t>
-  </si>
-  <si>
-    <t>TipoFalla</t>
-  </si>
-  <si>
-    <t>VEHICULO_VIAJABA_CLASIFICADO</t>
-  </si>
-  <si>
-    <t>Dia</t>
-  </si>
-  <si>
-    <t>Oficina</t>
-  </si>
-  <si>
-    <t>GravedadCod</t>
-  </si>
-  <si>
-    <t>GravedadNombre</t>
-  </si>
-  <si>
-    <t>ClaseCodigo</t>
-  </si>
-  <si>
-    <t>ClaseNombre</t>
-  </si>
-  <si>
-    <t>ChoqueCodigo</t>
-  </si>
-  <si>
-    <t>ChoqueNombre</t>
-  </si>
-  <si>
-    <t>ObjetoFijoCodigo</t>
-  </si>
-  <si>
-    <t>ObjetoFijoNombre</t>
-  </si>
-  <si>
-    <t>OtraClase</t>
-  </si>
-  <si>
-    <t>NombreOtraClase</t>
-  </si>
-  <si>
-    <t>Latitud</t>
-  </si>
-  <si>
-    <t>Longitud</t>
-  </si>
-  <si>
-    <t>Direccion</t>
-  </si>
-  <si>
-    <t>TipoVia1</t>
-  </si>
-  <si>
-    <t>NumeroVia1</t>
-  </si>
-  <si>
-    <t>LetraVia1</t>
-  </si>
-  <si>
-    <t>CardinalVia1</t>
-  </si>
-  <si>
-    <t>TipoVia2</t>
-  </si>
-  <si>
-    <t>NumeroVia2</t>
-  </si>
-  <si>
-    <t>LetraVia2</t>
-  </si>
-  <si>
-    <t>CardinalVia2</t>
-  </si>
-  <si>
-    <t>Complemento</t>
-  </si>
-  <si>
-    <t>Municipio</t>
-  </si>
-  <si>
-    <t>Localidad</t>
-  </si>
-  <si>
-    <t>FechaOcurrencia</t>
-  </si>
-  <si>
-    <t>HoraOcurrencia</t>
-  </si>
-  <si>
-    <t>HORA_PROCESADA</t>
-  </si>
-  <si>
-    <t>Sector</t>
-  </si>
-  <si>
-    <t>Zona</t>
-  </si>
-  <si>
-    <t>TipoDisenno</t>
-  </si>
-  <si>
-    <t>TipoTiempo</t>
-  </si>
-  <si>
-    <t>ZonaTransito</t>
-  </si>
-  <si>
-    <t>AreaTransito</t>
-  </si>
-  <si>
-    <t>CON_BICICLETA</t>
-  </si>
-  <si>
-    <t>CON_CARGA</t>
-  </si>
-  <si>
-    <t>CON_EMBRIAGUEZ</t>
-  </si>
-  <si>
-    <t>CON_HUECOS</t>
-  </si>
-  <si>
-    <t>CON_MENORES</t>
-  </si>
-  <si>
-    <t>CON_MOTO</t>
-  </si>
-  <si>
-    <t>CON_PEATON</t>
-  </si>
-  <si>
-    <t>CON_PERSONA_MAYOR</t>
-  </si>
-  <si>
-    <t>CON_RUTAS</t>
-  </si>
-  <si>
-    <t>CON_TPI</t>
-  </si>
-  <si>
-    <t>CON_VELOCIDAD</t>
+    <t>* Tabla ACCIDENTES_AGG</t>
+  </si>
+  <si>
+    <t>* IdFormulario</t>
+  </si>
+  <si>
+    <t>* GravedadAccidente (GravedadCod)</t>
+  </si>
+  <si>
+    <t>* CumpleNormasSeguridad (lleva_*)</t>
+  </si>
+  <si>
+    <t>* TipoAccidente ( GravedadNombre y OtraClase )</t>
+  </si>
+  <si>
+    <t>* ChoqueNombre ( ChoqueNombre y ObjetoFijoNombre )</t>
+  </si>
+  <si>
+    <t>* Latitud</t>
+  </si>
+  <si>
+    <t>* Longitud</t>
+  </si>
+  <si>
+    <t>* HoraOcurrencia</t>
+  </si>
+  <si>
+    <t>* TipoVia (TipoTiempo)</t>
+  </si>
+  <si>
+    <t>* CantidadConductores</t>
+  </si>
+  <si>
+    <t>* CantidadBicicletas</t>
+  </si>
+  <si>
+    <t>* CantidadMotos</t>
+  </si>
+  <si>
+    <t>* CantidadLiviano</t>
+  </si>
+  <si>
+    <t>* CantidadPesados</t>
+  </si>
+  <si>
+    <t>* CantidadConductoresHombres</t>
+  </si>
+  <si>
+    <t>* CantidadConductoresMujeres</t>
+  </si>
+  <si>
+    <t>* MenorModeloVehiculoInvolucrado (ModeloVehiculo)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -399,12 +539,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Courier New"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="5">
@@ -445,7 +579,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -462,9 +596,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -619,7 +750,7 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>790575</xdr:colOff>
+      <xdr:colOff>788670</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
@@ -627,7 +758,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>2552700</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -642,8 +773,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="20648295" y="1066800"/>
-          <a:ext cx="1762125" cy="308610"/>
+          <a:off x="8539639" y="1045369"/>
+          <a:ext cx="1764030" cy="296227"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -679,21 +810,8 @@
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>Fechas</a:t>
+            <a:t>CONDUCTORES_AGG</a:t>
           </a:r>
-          <a:r>
-            <a:rPr lang="es-CO" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> en Beneficios</a:t>
-          </a:r>
-          <a:endParaRPr lang="es-CO" sz="1100">
-            <a:solidFill>
-              <a:srgbClr val="FF0000"/>
-            </a:solidFill>
-          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -702,15 +820,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>790575</xdr:colOff>
+      <xdr:colOff>788670</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>125730</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -727,8 +845,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="4655820" y="1211580"/>
-          <a:ext cx="1575435" cy="9525"/>
+          <a:off x="6974681" y="1185863"/>
+          <a:ext cx="1564958" cy="11430"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -757,15 +875,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>158116</xdr:colOff>
+      <xdr:colOff>160021</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>2857</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>3375660</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
+      <xdr:colOff>3371850</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>154781</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -780,8 +898,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5598796" y="2014537"/>
-          <a:ext cx="3217544" cy="1338263"/>
+          <a:off x="7910990" y="1967388"/>
+          <a:ext cx="3211829" cy="1223487"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -851,15 +969,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>697230</xdr:colOff>
+      <xdr:colOff>170497</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>118585</xdr:rowOff>
+      <xdr:rowOff>72865</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>2758440</xdr:colOff>
+      <xdr:colOff>3298031</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>80961</xdr:rowOff>
+      <xdr:rowOff>35241</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -874,8 +992,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6126480" y="4226241"/>
-          <a:ext cx="2061210" cy="319564"/>
+          <a:off x="7921466" y="4180521"/>
+          <a:ext cx="3127534" cy="319564"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -906,7 +1024,23 @@
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>T4. Obtener el día de la fecha</a:t>
+            <a:t>T4. Eliminar</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> registros con todos los Lleva_* vacíos</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -916,15 +1050,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>525781</xdr:colOff>
+      <xdr:colOff>535782</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>119538</xdr:rowOff>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>3006091</xdr:colOff>
+      <xdr:colOff>3017997</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>180498</xdr:rowOff>
+      <xdr:rowOff>71437</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -942,8 +1076,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5802631" y="3377088"/>
-          <a:ext cx="2480310" cy="241935"/>
+          <a:off x="8286751" y="3228975"/>
+          <a:ext cx="2482215" cy="235743"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -974,21 +1108,8 @@
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>T2.  Convertir</a:t>
+            <a:t>T2.  </a:t>
           </a:r>
-          <a:r>
-            <a:rPr lang="es-CO" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> la fecha a formato Date</a:t>
-          </a:r>
-          <a:endParaRPr lang="es-CO" sz="1100">
-            <a:solidFill>
-              <a:srgbClr val="FF0000"/>
-            </a:solidFill>
-          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1052,7 +1173,7 @@
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>T5. Obtener el mes de la fecha</a:t>
+            <a:t>T5.  </a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1117,7 +1238,7 @@
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>T6. Obtener el año de la fecha</a:t>
+            <a:t>T6. </a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1235,21 +1356,8 @@
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>T7. Eliminar</a:t>
+            <a:t>T7. </a:t>
           </a:r>
-          <a:r>
-            <a:rPr lang="es-CO" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> duplicados en ID tras estandarización</a:t>
-          </a:r>
-          <a:endParaRPr lang="es-CO" sz="1100">
-            <a:solidFill>
-              <a:srgbClr val="FF0000"/>
-            </a:solidFill>
-          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1258,15 +1366,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>440531</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>31911</xdr:rowOff>
+      <xdr:colOff>436721</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>137163</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>3098006</xdr:colOff>
+      <xdr:colOff>3101816</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>85251</xdr:rowOff>
+      <xdr:rowOff>15719</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1284,8 +1392,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5869781" y="3603786"/>
-          <a:ext cx="2657475" cy="589121"/>
+          <a:off x="8187690" y="3530444"/>
+          <a:ext cx="2665095" cy="592931"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -1316,7 +1424,7 @@
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>T3.  Hacer un full outter join</a:t>
+            <a:t>T3.  Eliminar</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="es-CO" sz="1100" baseline="0">
@@ -1324,7 +1432,7 @@
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t> de las fuentes originales con el id corregido</a:t>
+            <a:t> conductores con sexo SIN INFORMACION</a:t>
           </a:r>
           <a:endParaRPr lang="es-CO" sz="1100">
             <a:solidFill>
@@ -1394,21 +1502,8 @@
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>T8. Renombrar</a:t>
+            <a:t>T8. </a:t>
           </a:r>
-          <a:r>
-            <a:rPr lang="es-CO" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> columnas</a:t>
-          </a:r>
-          <a:endParaRPr lang="es-CO" sz="1100">
-            <a:solidFill>
-              <a:srgbClr val="FF0000"/>
-            </a:solidFill>
-          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1423,9 +1518,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>3063239</xdr:colOff>
+      <xdr:colOff>3067049</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1440,8 +1535,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="44660820" y="1066800"/>
-          <a:ext cx="2682239" cy="308610"/>
+          <a:off x="20883563" y="1045369"/>
+          <a:ext cx="2686049" cy="296227"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -1477,23 +1572,7 @@
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>Ids de Geografía</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-CO" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> y </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="es-CO" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Areas de Servicio</a:t>
+            <a:t>ACCIDENTES_AGG</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1503,7 +1582,7 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>2506980</xdr:colOff>
+      <xdr:colOff>2505075</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
@@ -1511,7 +1590,7 @@
       <xdr:col>10</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>125730</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1528,8 +1607,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="48547020" y="1211580"/>
-          <a:ext cx="1219200" cy="9525"/>
+          <a:off x="19661981" y="1185863"/>
+          <a:ext cx="1221582" cy="11430"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1558,13 +1637,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>1722120</xdr:colOff>
+      <xdr:colOff>1724025</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>1737360</xdr:colOff>
+      <xdr:colOff>1733550</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -1583,8 +1662,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="46001940" y="1375410"/>
-          <a:ext cx="15240" cy="453390"/>
+          <a:off x="22226588" y="1341596"/>
+          <a:ext cx="9525" cy="444342"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2080,10 +2159,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L58"/>
+  <dimension ref="A1:L74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2098,7 +2177,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -2114,14 +2193,14 @@
     </row>
     <row r="3" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
       <c r="G3" s="10" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
@@ -2130,49 +2209,49 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="G5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="K5" s="5" t="s">
         <v>2</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="E6" s="4"/>
       <c r="G6" s="2" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="K6" s="4"/>
     </row>
@@ -2188,471 +2267,1145 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E8" s="4"/>
       <c r="G8" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K8" s="4"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="2"/>
+        <v>15</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="C9" s="2" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="C10" s="2" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="2"/>
+        <v>16</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="C11" s="2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>11</v>
+        <v>4</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="2"/>
+        <v>17</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="C12" s="2" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="E12" s="4"/>
+      <c r="G12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="K12" s="4"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" s="2"/>
+        <v>84</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="C13" s="2" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="E13" s="4"/>
+      <c r="G13" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="K13" s="4"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="2"/>
+        <v>18</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="C14" s="2" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="E14" s="4"/>
+      <c r="G14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="K14" s="4"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" s="2"/>
+        <v>19</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="C15" s="2" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="E15" s="4"/>
+      <c r="G15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="K15" s="4"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" s="2"/>
+        <v>20</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="C16" s="2" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="E16" s="4"/>
+      <c r="G16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="K16" s="4"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="C17" s="2" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="E17" s="4"/>
+      <c r="G17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="K17" s="4"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" s="2"/>
+        <v>22</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>93</v>
+      </c>
       <c r="C18" s="2" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="E18" s="4"/>
+      <c r="G18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B19" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>94</v>
+      </c>
       <c r="C19" s="2" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="E19" s="4"/>
+      <c r="G19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" s="2"/>
+        <v>85</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="C20" s="2" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="E20" s="4"/>
+      <c r="G20" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="K20" s="5" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="C21" s="2" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="E21" s="4"/>
+      <c r="G21" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="K21" s="6" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" s="2"/>
+        <v>87</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>85</v>
+      </c>
       <c r="C22" s="2" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="E22" s="4"/>
+      <c r="G22" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="K22" s="8" t="s">
-        <v>16</v>
+        <v>131</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B23" s="2"/>
+        <v>88</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>86</v>
+      </c>
       <c r="C23" s="2" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="E23" s="4"/>
+      <c r="G23" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="K23" s="6"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B24" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>87</v>
+      </c>
       <c r="C24" s="2" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="E24" s="4"/>
+      <c r="G24" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="K24" s="6" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B25" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="C25" s="2" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="E25" s="4"/>
+      <c r="G25" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="K25" s="8" t="s">
-        <v>9</v>
+        <v>132</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B26" s="2"/>
+        <v>26</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="C26" s="2" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="E26" s="4"/>
+      <c r="G26" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="K26" s="8" t="s">
-        <v>10</v>
+        <v>135</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B27" s="2"/>
+        <v>89</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="C27" s="2" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="E27" s="4"/>
+      <c r="G27" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K27" s="8" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B28" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="C28" s="2" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="E28" s="4"/>
+      <c r="G28" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K28" s="8" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B29" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="C29" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E29" s="4"/>
+      <c r="G29" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H29" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E29" s="4"/>
+      <c r="I29" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="K29" s="8" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B30" s="2"/>
+        <v>29</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="C30" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E30" s="4"/>
+      <c r="G30" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H30" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E30" s="4"/>
+      <c r="I30" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K30" s="8" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B31" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="C31" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E31" s="4"/>
+      <c r="G31" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H31" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E31" s="4"/>
+      <c r="I31" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="K31" s="8" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B32" s="2"/>
+        <v>31</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="C32" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E32" s="4"/>
+      <c r="G32" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H32" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E32" s="4"/>
-    </row>
-    <row r="33" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="I32" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="K32" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="C33" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E33" s="4"/>
+      <c r="G33" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H33" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E33" s="4"/>
-    </row>
-    <row r="34" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="I33" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="K33" s="8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="C34" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E34" s="4"/>
+      <c r="G34" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H34" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E34" s="4"/>
-    </row>
-    <row r="35" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="I34" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="K34" s="8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="C35" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E35" s="4"/>
+      <c r="G35" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H35" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E35" s="4"/>
-    </row>
-    <row r="36" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="I35" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="K35" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="C36" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H36" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="37" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="I36" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K36" s="8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="C37" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H37" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="38" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="I37" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K37" s="8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="C38" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H38" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E38" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="39" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="I38" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="K38" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>83</v>
+      </c>
       <c r="C39" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H39" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E39" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="40" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="I39" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="K39" s="8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="C40" s="2" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="41" spans="3:5" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="K40" s="8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="C41" s="2" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="E41" s="6"/>
-    </row>
-    <row r="42" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G41" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K41" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="C42" s="2" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="43" spans="3:5" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="K42" s="8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="C43" s="2" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="44" spans="3:5" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I43" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K43" s="8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="C44" s="2" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="45" spans="3:5" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K44" s="8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="C45" s="2" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="46" spans="3:5" x14ac:dyDescent="0.3">
+        <v>134</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="K45" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="C46" s="2" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="47" spans="3:5" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K46" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="C47" s="2" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="E47" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="48" spans="3:5" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I47" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K47" s="8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="C48" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+      <c r="E48" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="K48" s="8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="C49" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+      <c r="E49" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="K49" s="8" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
+        <v>83</v>
+      </c>
       <c r="C50" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+      <c r="E50" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="I50" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="K50" s="8" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C51" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+      <c r="E51" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="I51" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="K51" s="8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C52" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="I52" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="K52" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C53" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+      <c r="E53" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="I53" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="K53" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C54" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="I54" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="K54" s="8" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C55" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="I55" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K55" s="8" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C56" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+      <c r="E56" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="I56" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C57" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+      <c r="E57" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="I57" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C58" s="2" t="s">
-        <v>101</v>
+        <v>83</v>
+      </c>
+      <c r="E58" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="I58" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E59" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E60" s="8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E61" s="8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E62" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E63" s="8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E64" s="8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="65" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E65" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="66" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E66" s="8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="67" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E67" s="8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="68" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E68" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="69" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E69" s="8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="70" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E70" s="8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="71" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E71" s="8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="72" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E72" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="73" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E73" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="74" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E74" s="8" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -2667,453 +3420,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E415AA4-BD60-4900-91F5-7BAE20623888}">
-  <dimension ref="A1:F24"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="11"/>
-      <c r="B1">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1">
-        <v>66179</v>
-      </c>
-      <c r="E1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="11"/>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2">
-        <v>66179</v>
-      </c>
-      <c r="E2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="11"/>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3">
-        <v>66179</v>
-      </c>
-      <c r="E3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="11"/>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4">
-        <v>66179</v>
-      </c>
-      <c r="E4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="11"/>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5">
-        <v>66179</v>
-      </c>
-      <c r="E5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="11"/>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6">
-        <v>66179</v>
-      </c>
-      <c r="E6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="11"/>
-      <c r="B7">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7">
-        <v>66179</v>
-      </c>
-      <c r="E7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="11"/>
-      <c r="B8">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8">
-        <v>66179</v>
-      </c>
-      <c r="E8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="11"/>
-      <c r="B9">
-        <v>8</v>
-      </c>
-      <c r="C9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9">
-        <v>66179</v>
-      </c>
-      <c r="E9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="11"/>
-      <c r="B10">
-        <v>9</v>
-      </c>
-      <c r="C10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10">
-        <v>66179</v>
-      </c>
-      <c r="E10" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="11"/>
-      <c r="B11">
-        <v>10</v>
-      </c>
-      <c r="C11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11">
-        <v>66179</v>
-      </c>
-      <c r="E11" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="11"/>
-      <c r="B12">
-        <v>11</v>
-      </c>
-      <c r="C12" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12">
-        <v>66179</v>
-      </c>
-      <c r="E12" t="s">
-        <v>29</v>
-      </c>
-      <c r="F12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="11"/>
-      <c r="B13">
-        <v>12</v>
-      </c>
-      <c r="C13" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13">
-        <v>66179</v>
-      </c>
-      <c r="E13" t="s">
-        <v>29</v>
-      </c>
-      <c r="F13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="11"/>
-      <c r="B14">
-        <v>13</v>
-      </c>
-      <c r="C14" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14">
-        <v>66179</v>
-      </c>
-      <c r="E14" t="s">
-        <v>29</v>
-      </c>
-      <c r="F14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="11"/>
-      <c r="B15">
-        <v>14</v>
-      </c>
-      <c r="C15" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15">
-        <v>66179</v>
-      </c>
-      <c r="E15" t="s">
-        <v>29</v>
-      </c>
-      <c r="F15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="11"/>
-      <c r="B16">
-        <v>15</v>
-      </c>
-      <c r="C16" t="s">
-        <v>46</v>
-      </c>
-      <c r="D16">
-        <v>66179</v>
-      </c>
-      <c r="E16" t="s">
-        <v>29</v>
-      </c>
-      <c r="F16" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="11"/>
-      <c r="B17">
-        <v>16</v>
-      </c>
-      <c r="C17" t="s">
-        <v>48</v>
-      </c>
-      <c r="D17">
-        <v>66179</v>
-      </c>
-      <c r="E17" t="s">
-        <v>29</v>
-      </c>
-      <c r="F17" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="11"/>
-      <c r="B18">
-        <v>17</v>
-      </c>
-      <c r="C18" t="s">
-        <v>49</v>
-      </c>
-      <c r="D18">
-        <v>66179</v>
-      </c>
-      <c r="E18" t="s">
-        <v>29</v>
-      </c>
-      <c r="F18" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="11"/>
-      <c r="B19">
-        <v>18</v>
-      </c>
-      <c r="C19" t="s">
-        <v>50</v>
-      </c>
-      <c r="D19">
-        <v>66179</v>
-      </c>
-      <c r="E19" t="s">
-        <v>29</v>
-      </c>
-      <c r="F19" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="11"/>
-      <c r="B20">
-        <v>19</v>
-      </c>
-      <c r="C20" t="s">
-        <v>51</v>
-      </c>
-      <c r="D20">
-        <v>66179</v>
-      </c>
-      <c r="E20" t="s">
-        <v>29</v>
-      </c>
-      <c r="F20" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="11"/>
-      <c r="B21">
-        <v>20</v>
-      </c>
-      <c r="C21" t="s">
-        <v>52</v>
-      </c>
-      <c r="D21">
-        <v>66179</v>
-      </c>
-      <c r="E21" t="s">
-        <v>29</v>
-      </c>
-      <c r="F21" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="11"/>
-      <c r="B22">
-        <v>21</v>
-      </c>
-      <c r="C22" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22">
-        <v>66179</v>
-      </c>
-      <c r="E22" t="s">
-        <v>29</v>
-      </c>
-      <c r="F22" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="11"/>
-      <c r="B23">
-        <v>22</v>
-      </c>
-      <c r="C23" t="s">
-        <v>54</v>
-      </c>
-      <c r="D23">
-        <v>66179</v>
-      </c>
-      <c r="E23" t="s">
-        <v>29</v>
-      </c>
-      <c r="F23" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="11"/>
-      <c r="B24">
-        <v>23</v>
-      </c>
-      <c r="C24" t="s">
-        <v>55</v>
-      </c>
-      <c r="D24">
-        <v>66179</v>
-      </c>
-      <c r="E24" t="s">
-        <v>29</v>
-      </c>
-      <c r="F24" t="s">
-        <v>33</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -3121,6 +3427,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A7ADC6895240034186F3B406871EEF02" ma:contentTypeVersion="2" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="21f6a9d752a9557c812eac8992c72391">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="403983a5-8176-495f-8017-1cc5516bc8be" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="50973fac330fa9540a57dc818ca860e2" ns2:_="">
     <xsd:import namespace="403983a5-8176-495f-8017-1cc5516bc8be"/>
@@ -3252,15 +3567,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B5F6310-4DBD-40BF-94B5-6E3A281422E0}">
   <ds:schemaRefs>
@@ -3271,6 +3577,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67B34AF8-AC51-4236-BB98-0DF28490C8EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03D42706-7B6F-4C75-8FFF-22DDC41CD9AE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3286,12 +3600,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67B34AF8-AC51-4236-BB98-0DF28490C8EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>